<commit_message>
add test data and test case for left to right sorting with 3 columns
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/excelsortsample.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/excelsortsample.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="285" windowWidth="18795" windowHeight="10485"/>
+    <workbookView xWindow="600" yWindow="285" windowWidth="18795" windowHeight="10485" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SampleData" sheetId="1" r:id="rId1"/>
     <sheet name="WeekdaySort" sheetId="7" r:id="rId2"/>
     <sheet name="MonthData" sheetId="4" r:id="rId3"/>
     <sheet name="SortIcons" sheetId="9" r:id="rId4"/>
-    <sheet name="MyLinks" sheetId="8" r:id="rId5"/>
+    <sheet name="Left2Right" sheetId="8" r:id="rId5"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
@@ -20,12 +20,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MonthData!$A$1:$G$6</definedName>
     <definedName name="Product">[1]Prices!$B$2:$B$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -198,33 +198,6 @@
     <t>Region</t>
   </si>
   <si>
-    <t>Contextures Links</t>
-  </si>
-  <si>
-    <t>Contextures Excel Tips Website</t>
-  </si>
-  <si>
-    <t>Contextures Excel Blog</t>
-  </si>
-  <si>
-    <t>Excel Pivot Tables Blog</t>
-  </si>
-  <si>
-    <t>Debra's Pivot Table Books on Amazon</t>
-  </si>
-  <si>
-    <t>Contextures Recommends</t>
-  </si>
-  <si>
-    <t>Jon Peltier's Excel Chart Utilities</t>
-  </si>
-  <si>
-    <t>ExcelUser Dashboards</t>
-  </si>
-  <si>
-    <t>Chandoo's Project Management Templates</t>
-  </si>
-  <si>
     <t>www.contextures.com</t>
   </si>
   <si>
@@ -259,18 +232,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>30 Excel Functions in 30 Days eBook Kit</t>
-  </si>
-  <si>
-    <t>PivotPower Premium Add-in</t>
-  </si>
-  <si>
-    <t>Excel Courses Online</t>
-  </si>
-  <si>
-    <t>Chandoo's Excel VBA School</t>
   </si>
   <si>
     <t>Product</t>
@@ -300,15 +261,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="180" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,14 +287,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -351,14 +312,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -371,13 +332,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -385,7 +340,7 @@
       <u/>
       <sz val="11"/>
       <color indexed="12"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -399,7 +354,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -445,10 +400,10 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
@@ -460,15 +415,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -477,34 +432,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 2 2" xfId="7"/>
     <cellStyle name="Normal 2 3 2" xfId="5"/>
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="千分位" xfId="3" builtinId="3"/>
-    <cellStyle name="貨幣" xfId="4" builtinId="4"/>
-    <cellStyle name="超連結" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -523,7 +480,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -547,7 +504,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -571,7 +528,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -595,7 +552,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -619,7 +576,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="180" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -643,7 +600,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -667,7 +624,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="179" formatCode="[$-409]d\-mmm;@"/>
+      <numFmt numFmtId="167" formatCode="[$-409]d\-mmm;@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -691,7 +648,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="179" formatCode="[$-409]d\-mmm;@"/>
+      <numFmt numFmtId="167" formatCode="[$-409]d\-mmm;@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -744,7 +701,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -760,7 +717,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Orders"/>
@@ -840,7 +797,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -914,7 +871,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -949,7 +905,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1125,15 +1080,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
@@ -1146,7 +1101,7 @@
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1171,11 +1126,9 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1201,7 +1154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1227,7 +1180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1253,7 +1206,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1279,7 +1232,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1305,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1331,7 +1284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1357,7 +1310,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1383,7 +1336,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1409,7 +1362,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1439,14 +1392,14 @@
   <sortState ref="A2:H1001">
     <sortCondition ref="A2"/>
   </sortState>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -1454,7 +1407,7 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="8.140625" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="11" customWidth="1"/>
@@ -1462,29 +1415,29 @@
     <col min="4" max="4" width="12.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21">
       <c r="A1" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="7">
         <v>40550</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>676</v>
@@ -1494,12 +1447,12 @@
         <v>1210.04</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="7">
         <v>40555</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>552</v>
@@ -1509,12 +1462,12 @@
         <v>988.08</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="7">
         <v>40601</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C4">
         <v>571</v>
@@ -1524,12 +1477,12 @@
         <v>1022.09</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="7">
         <v>40615</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>170</v>
@@ -1539,12 +1492,12 @@
         <v>304.3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="7">
         <v>40615</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C6">
         <v>311</v>
@@ -1554,12 +1507,12 @@
         <v>556.69000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="7">
         <v>40630</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C7">
         <v>335</v>
@@ -1569,12 +1522,12 @@
         <v>599.65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="7">
         <v>40647</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>123</v>
@@ -1584,12 +1537,12 @@
         <v>220.17000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="7">
         <v>40648</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>366</v>
@@ -1599,12 +1552,12 @@
         <v>655.14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="7">
         <v>40648</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>461</v>
@@ -1614,12 +1567,12 @@
         <v>825.19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="7">
         <v>40690</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>244</v>
@@ -1629,12 +1582,12 @@
         <v>436.76</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="7">
         <v>40692</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C12">
         <v>600</v>
@@ -1644,12 +1597,12 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="7">
         <v>40720</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>253</v>
@@ -1659,12 +1612,12 @@
         <v>452.87</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6">
       <c r="A14" s="7">
         <v>40723</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C14">
         <v>156</v>
@@ -1674,12 +1627,12 @@
         <v>279.24</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="7">
         <v>40762</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C15">
         <v>591</v>
@@ -1689,12 +1642,12 @@
         <v>1057.8900000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6">
       <c r="A16" s="7">
         <v>40786</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>140</v>
@@ -1704,12 +1657,12 @@
         <v>250.6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="7">
         <v>40882</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C17">
         <v>591</v>
@@ -1719,12 +1672,12 @@
         <v>1057.8900000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="7">
         <v>40884</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C18">
         <v>617</v>
@@ -1734,12 +1687,12 @@
         <v>1104.43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="7">
         <v>40886</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C19">
         <v>179</v>
@@ -1749,12 +1702,12 @@
         <v>320.41000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="7">
         <v>40902</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C20">
         <v>235</v>
@@ -1768,26 +1721,26 @@
   <sortState ref="A2:D20">
     <sortCondition ref="A2"/>
   </sortState>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="7" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
@@ -1810,7 +1763,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" s="16" t="s">
         <v>51</v>
       </c>
@@ -1833,7 +1786,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" s="16" t="s">
         <v>46</v>
       </c>
@@ -1856,7 +1809,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" s="16" t="s">
         <v>50</v>
       </c>
@@ -1879,7 +1832,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
@@ -1902,9 +1855,9 @@
         <v>562</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="21.75" customHeight="1" thickBot="1">
       <c r="A6" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B6" s="13">
         <f t="shared" ref="B6:G6" si="0">SUM(B2:B5)</f>
@@ -1931,305 +1884,305 @@
         <v>3455</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="17.25" thickTop="1"/>
+    <row r="9" spans="1:7">
       <c r="A9" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="21">
       <c r="A12" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <sortState columnSort="1" ref="B1:G6">
     <sortCondition ref="B1:G1" customList="Jan,Feb,Mar,Apr,May,Jun,Jul,Aug,Sep,Oct,Nov,Dec"/>
   </sortState>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="26">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="25">
         <v>41426</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="28">
+      <c r="C2" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="27">
         <v>10</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="26">
         <f>VLOOKUP(C2,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>12.95</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <f t="shared" ref="F2:F9" si="0">D2*E2</f>
         <v>129.5</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="26">
         <f t="shared" ref="G2:G9" si="1">F2*0.07</f>
         <v>9.0650000000000013</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="26">
         <f t="shared" ref="H2:H9" si="2">SUM(F2:G2)</f>
         <v>138.565</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="26">
+    <row r="3" spans="1:8">
+      <c r="A3" s="25">
         <v>41427</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="28">
+      <c r="C3" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="27">
         <v>15</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <f>VLOOKUP(C3,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>12.95</v>
       </c>
-      <c r="F3" s="29">
+      <c r="F3" s="28">
         <f t="shared" si="0"/>
         <v>194.25</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="26">
         <f t="shared" si="1"/>
         <v>13.597500000000002</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="26">
         <f t="shared" si="2"/>
         <v>207.8475</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="26">
+    <row r="4" spans="1:8">
+      <c r="A4" s="25">
         <v>41428</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="28">
+      <c r="C4" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="27">
         <v>25</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <f>VLOOKUP(C4,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>2.19</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="28">
         <f t="shared" si="0"/>
         <v>54.75</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="26">
         <f t="shared" si="1"/>
         <v>3.8325000000000005</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="26">
         <f t="shared" si="2"/>
         <v>58.582500000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="26">
+    <row r="5" spans="1:8">
+      <c r="A5" s="25">
         <v>41429</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="28">
+      <c r="C5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="27">
         <v>30</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <f>VLOOKUP(C5,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>2.19</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="28">
         <f t="shared" si="0"/>
         <v>65.7</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <f t="shared" si="1"/>
         <v>4.5990000000000002</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="26">
         <f t="shared" si="2"/>
         <v>70.299000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="26">
+    <row r="6" spans="1:8">
+      <c r="A6" s="25">
         <v>41430</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D6" s="28">
+      <c r="C6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="27">
         <v>40</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <f>VLOOKUP(C6,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>12.95</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <f t="shared" si="0"/>
         <v>518</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <f t="shared" si="1"/>
         <v>36.260000000000005</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <f t="shared" si="2"/>
         <v>554.26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="26">
+    <row r="7" spans="1:8">
+      <c r="A7" s="25">
         <v>41431</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="28">
+      <c r="C7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="27">
         <v>50</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <f>VLOOKUP(C7,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>12.95</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="28">
         <f t="shared" si="0"/>
         <v>647.5</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <f t="shared" si="1"/>
         <v>45.325000000000003</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <f t="shared" si="2"/>
         <v>692.82500000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="26">
+    <row r="8" spans="1:8">
+      <c r="A8" s="25">
         <v>41432</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="28">
+      <c r="C8" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="27">
         <v>20</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="26">
         <v>15.95</v>
       </c>
-      <c r="F8" s="29">
+      <c r="F8" s="28">
         <f t="shared" si="0"/>
         <v>319</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <f t="shared" si="1"/>
         <v>22.330000000000002</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="26">
         <f t="shared" si="2"/>
         <v>341.33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="26">
+    <row r="9" spans="1:8">
+      <c r="A9" s="25">
         <v>41433</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="28">
+      <c r="C9" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="27">
         <v>18</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="26">
         <f>VLOOKUP(C9,[1]Prices!$B$2:$C$5,2,FALSE)</f>
         <v>2.19</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <f t="shared" si="0"/>
         <v>39.42</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="26">
         <f t="shared" si="1"/>
         <v>2.7594000000000003</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="26">
         <f t="shared" si="2"/>
         <v>42.179400000000001</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="D2:D9">
     <cfRule type="iconSet" priority="1">
       <iconSet>
@@ -2252,19 +2205,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:B18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="256" width="9.140625" style="4"/>
+    <col min="1" max="1" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="11.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="11.7109375" style="4" customWidth="1"/>
+    <col min="12" max="256" width="9.140625" style="4"/>
     <col min="257" max="257" width="3" style="4" customWidth="1"/>
     <col min="258" max="258" width="41.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="259" max="512" width="9.140625" style="4"/>
@@ -2456,121 +2411,295 @@
     <col min="16131" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="21" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30">
+        <v>2</v>
+      </c>
+      <c r="D1" s="30">
+        <v>3</v>
+      </c>
+      <c r="E1" s="30">
+        <v>4</v>
+      </c>
+      <c r="F1" s="30">
+        <v>5</v>
+      </c>
+      <c r="G1" s="30">
+        <v>6</v>
+      </c>
+      <c r="H1" s="30">
+        <v>7</v>
+      </c>
+      <c r="I1" s="30">
+        <v>8</v>
+      </c>
+      <c r="J1" s="30">
+        <v>9</v>
+      </c>
+      <c r="K1" s="30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="30">
+        <v>1943</v>
+      </c>
+      <c r="C4" s="30">
+        <v>1945</v>
+      </c>
+      <c r="D4" s="30">
+        <v>1982</v>
+      </c>
+      <c r="E4" s="30">
+        <v>1975</v>
+      </c>
+      <c r="F4" s="30">
+        <v>1991</v>
+      </c>
+      <c r="G4" s="30">
+        <v>1985</v>
+      </c>
+      <c r="H4" s="30">
+        <v>1975</v>
+      </c>
+      <c r="I4" s="30">
+        <v>1959</v>
+      </c>
+      <c r="J4" s="30">
+        <v>1980</v>
+      </c>
+      <c r="K4" s="30">
+        <v>1967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="17"/>
-      <c r="B8" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="17"/>
-      <c r="B9" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" ht="18.75">
       <c r="A10" s="17"/>
-      <c r="B10" s="22"/>
-    </row>
-    <row r="11" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" ht="6" customHeight="1">
       <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="17"/>
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="20"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="17"/>
-      <c r="B13" s="21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="20"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="17"/>
-      <c r="B14" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="19"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="17"/>
-      <c r="B15" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="24"/>
+      <c r="B15" s="20"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="22"/>
+      <c r="B16" s="20"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="23"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="B7" r:id="rId3"/>
-    <hyperlink ref="B13" r:id="rId4" tooltip="Jon Peltier's Excel Chart Utilities"/>
-    <hyperlink ref="B14" r:id="rId5" tooltip="ExcelUser Dashboards"/>
-    <hyperlink ref="B17" r:id="rId6" tooltip="Chandoo's Project Management Templates"/>
-    <hyperlink ref="B9" r:id="rId7" tooltip="Debra's Pivot Table Books on Amazon"/>
-    <hyperlink ref="B5" r:id="rId8" tooltip="30 Excel Functions in 30 Days eBook kit"/>
-    <hyperlink ref="B16" r:id="rId9" tooltip="Chandoo's Excel VBA School"/>
-    <hyperlink ref="B4" r:id="rId10" tooltip="PivotPower Premium Add-in"/>
-    <hyperlink ref="B15" r:id="rId11" tooltip="Excel Courses Online"/>
-  </hyperlinks>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;Lwww.contextures.com&amp;R&amp;D</oddFooter>
   </headerFooter>

</xml_diff>